<commit_message>
fixed some bugs. 2021/04/06 22:25
</commit_message>
<xml_diff>
--- a/res/SEED_IV/result.xlsx
+++ b/res/SEED_IV/result.xlsx
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4931</v>
+        <v>0.7621</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.9043</v>
       </c>
     </row>
     <row r="4">
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.6504</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.9034</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.8723</v>
       </c>
     </row>
     <row r="7">
@@ -508,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.5569</v>
       </c>
     </row>
     <row r="8">
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.6069</v>
       </c>
     </row>
     <row r="9">
@@ -530,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.7092000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -541,7 +541,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.7276</v>
       </c>
     </row>
     <row r="11">
@@ -552,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.7517</v>
       </c>
     </row>
     <row r="12">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.4752</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
new results. 2021/04/08 12:32
</commit_message>
<xml_diff>
--- a/res/SEED_IV/result.xlsx
+++ b/res/SEED_IV/result.xlsx
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4752</v>
+        <v>0.5816</v>
       </c>
     </row>
     <row r="13">
@@ -574,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.7846</v>
       </c>
     </row>
     <row r="14">
@@ -585,7 +585,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.4931</v>
       </c>
     </row>
     <row r="15">
@@ -596,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.5071</v>
       </c>
     </row>
     <row r="16">
@@ -607,7 +607,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.8415</v>
       </c>
     </row>
     <row r="17">
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.7586000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -629,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.6773</v>
       </c>
     </row>
     <row r="19">
@@ -640,7 +640,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>0.7846</v>
       </c>
     </row>
     <row r="20">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.7586000000000001</v>
       </c>
     </row>
     <row r="21">
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.922</v>
       </c>
     </row>
     <row r="22">
@@ -673,7 +673,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>0.3943</v>
       </c>
     </row>
     <row r="23">
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.9552</v>
       </c>
     </row>
     <row r="24">
@@ -695,7 +695,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.8369</v>
       </c>
     </row>
     <row r="25">
@@ -706,7 +706,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.9228</v>
       </c>
     </row>
     <row r="26">
@@ -717,7 +717,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -728,7 +728,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>0.7695</v>
       </c>
     </row>
     <row r="28">
@@ -739,7 +739,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.7967</v>
       </c>
     </row>
     <row r="29">
@@ -750,7 +750,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>0.6414</v>
       </c>
     </row>
     <row r="30">
@@ -761,7 +761,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>0.6844</v>
       </c>
     </row>
     <row r="31">
@@ -772,7 +772,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.626</v>
       </c>
     </row>
     <row r="32">
@@ -783,7 +783,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.869</v>
       </c>
     </row>
     <row r="33">
@@ -794,7 +794,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.4965</v>
       </c>
     </row>
     <row r="34">
@@ -805,7 +805,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.7724</v>
       </c>
     </row>
     <row r="35">
@@ -816,7 +816,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>0.9517</v>
       </c>
     </row>
     <row r="36">
@@ -827,7 +827,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.3723</v>
       </c>
     </row>
     <row r="37">
@@ -838,7 +838,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>0.4675</v>
       </c>
     </row>
     <row r="38">
@@ -849,7 +849,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>0.6516999999999999</v>
       </c>
     </row>
     <row r="39">
@@ -860,7 +860,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>0.7589</v>
       </c>
     </row>
     <row r="40">
@@ -871,7 +871,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>0.4797</v>
       </c>
     </row>
     <row r="41">
@@ -882,7 +882,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>0.7171999999999999</v>
       </c>
     </row>
     <row r="42">
@@ -893,7 +893,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.9043</v>
       </c>
     </row>
     <row r="43">
@@ -904,7 +904,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.4024</v>
       </c>
     </row>
     <row r="44">
@@ -915,7 +915,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>0.5793</v>
       </c>
     </row>
     <row r="45">
@@ -926,7 +926,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>0.8723</v>
       </c>
     </row>
     <row r="46">
@@ -937,7 +937,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.7886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results, fixed some bugs. 2021/04/14 17:28
</commit_message>
<xml_diff>
--- a/res/SEED_IV/result.xlsx
+++ b/res/SEED_IV/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HANYIIK\Desktop\final_res\SEED_IV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\最新结果\SEED_IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEE95EC-2034-4553-B1A0-9EF2120B0B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753065D3-3426-40E6-86D4-C1528DAE913E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </si>
   <si>
     <t>平均</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -49,6 +49,13 @@
       <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -79,13 +86,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -139,16 +139,16 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -157,11 +157,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -472,14 +472,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="9.875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -518,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>0.90339999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -565,8 +562,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.77239999999999998</v>
+      <c r="B11" s="2">
+        <v>0.89659999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -598,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.84750000000000003</v>
+        <v>0.91839999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -606,7 +603,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.85770000000000002</v>
+        <v>0.90239999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -614,7 +611,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.85170000000000001</v>
+        <v>0.90339999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -638,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.90690000000000004</v>
+        <v>0.94830000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
@@ -646,7 +643,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.96809999999999996</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
@@ -654,7 +651,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4">
-        <v>0.5081</v>
+        <v>0.53659999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
@@ -717,8 +714,8 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>0.79079999999999995</v>
+      <c r="B30" s="2">
+        <v>0.85460000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
@@ -726,7 +723,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>0.626</v>
+        <v>0.67479999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
@@ -766,7 +763,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>0.4929</v>
+        <v>0.63829999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
@@ -782,7 +779,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.81720000000000004</v>
+        <v>0.88280000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
@@ -805,8 +802,8 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="3">
-        <v>0.75519999999999998</v>
+      <c r="B41" s="2">
+        <v>0.83789999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
@@ -822,15 +819,15 @@
         <v>42</v>
       </c>
       <c r="B43" s="4">
-        <v>0.40239999999999998</v>
+        <v>0.52849999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="4">
-        <v>0.57930000000000004</v>
+      <c r="B44" s="3">
+        <v>0.72760000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
@@ -838,15 +835,15 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>0.87229999999999996</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
-        <v>0.78859999999999997</v>
+      <c r="B46" s="2">
+        <v>0.83330000000000004</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
@@ -855,11 +852,11 @@
       </c>
       <c r="B47" s="5">
         <f>AVERAGE(B2:B46)</f>
-        <v>0.80607111111111129</v>
+        <v>0.83591555555555552</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>